<commit_message>
Loop detected and deleted
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1698,22 +1698,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C142" activeCellId="0" sqref="C142"/>
+      <selection pane="topLeft" activeCell="C143" activeCellId="0" sqref="C143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,7 +3185,7 @@
         <v>145</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Duplicates deleted from Sorted LL
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1704,11 +1704,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C143" activeCellId="0" sqref="C143"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B141" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C144" activeCellId="0" sqref="C144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
@@ -3196,7 +3196,7 @@
         <v>146</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Duplicates deleted from Unsorted LL
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1705,10 +1705,10 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B141" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C144" activeCellId="0" sqref="C144"/>
+      <selection pane="topLeft" activeCell="C146" activeCellId="0" sqref="C146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
@@ -3207,7 +3207,7 @@
         <v>147</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3218,7 +3218,7 @@
         <v>148</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Last Element to Front
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1704,8 +1704,8 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B141" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C146" activeCellId="0" sqref="C146"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B145" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C147" activeCellId="0" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3229,7 +3229,7 @@
         <v>149</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added 1 to LL considering it as number
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1704,11 +1704,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B147" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B147" activeCellId="0" sqref="B147"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C175" activeCellId="0" sqref="C175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
@@ -3240,7 +3240,7 @@
         <v>150</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added 1 to LL as a number Successfully
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1708,7 +1708,7 @@
       <selection pane="topLeft" activeCell="C175" activeCellId="0" sqref="C175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
@@ -3221,7 +3221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="6" t="s">
         <v>141</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="6" t="s">
         <v>141</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>150</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added 2 LL as a numbers
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1705,10 +1705,10 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C175" activeCellId="0" sqref="C175"/>
+      <selection pane="topLeft" activeCell="C149" activeCellId="0" sqref="C149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
@@ -3251,7 +3251,7 @@
         <v>151</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Intersection Point Found of 2 LL
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1705,7 +1705,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C149" activeCellId="0" sqref="C149"/>
+      <selection pane="topLeft" activeCell="C150" activeCellId="0" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3262,7 +3262,7 @@
         <v>152</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Intersection Point Found of 2 LLs
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1705,10 +1705,10 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C150" activeCellId="0" sqref="C150"/>
+      <selection pane="topLeft" activeCell="C151" activeCellId="0" sqref="C151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.71484375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.71875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
@@ -3273,7 +3273,7 @@
         <v>153</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Merge and Quick Sort Done
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1705,10 +1705,10 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C151" activeCellId="0" sqref="C151"/>
+      <selection pane="topLeft" activeCell="C153" activeCellId="0" sqref="C153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.71875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
@@ -3265,7 +3265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="6" t="s">
         <v>141</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="6" t="s">
         <v>141</v>
       </c>
@@ -3284,10 +3284,10 @@
         <v>154</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="6" t="s">
         <v>141</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>155</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Middle element found of LL
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1442,7 +1442,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1529,6 +1529,13 @@
       <family val="0"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1575,7 +1582,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1617,6 +1624,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1704,11 +1715,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C153" activeCellId="0" sqref="C153"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C154" activeCellId="0" sqref="C154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.73828125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
@@ -3283,8 +3294,8 @@
       <c r="B151" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C151" s="5" t="s">
-        <v>8</v>
+      <c r="C151" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3294,8 +3305,8 @@
       <c r="B152" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C152" s="5" t="s">
-        <v>8</v>
+      <c r="C152" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3306,7 +3317,7 @@
         <v>156</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4009,7 +4020,7 @@
       <c r="A220" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B220" s="11" t="s">
+      <c r="B220" s="12" t="s">
         <v>221</v>
       </c>
       <c r="C220" s="5" t="s">
@@ -4946,7 +4957,7 @@
       <c r="A309" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B309" s="11" t="s">
+      <c r="B309" s="12" t="s">
         <v>306</v>
       </c>
       <c r="C309" s="5" t="s">
@@ -5317,7 +5328,7 @@
       <c r="A344" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B344" s="11" t="s">
+      <c r="B344" s="12" t="s">
         <v>340</v>
       </c>
       <c r="C344" s="5" t="s">

</xml_diff>

<commit_message>
Checked LL is CLL or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C154" activeCellId="0" sqref="C154"/>
+      <selection pane="topLeft" activeCell="C155" activeCellId="0" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73828125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3328,7 +3328,7 @@
         <v>157</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Palindrome check of LL
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,10 +1716,10 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C156" activeCellId="0" sqref="C156"/>
+      <selection pane="topLeft" activeCell="C157" activeCellId="0" sqref="C157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73828125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.74609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
@@ -3350,7 +3350,7 @@
         <v>159</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Deleted node from CLL
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1715,8 +1715,8 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C157" activeCellId="0" sqref="C157"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C158" activeCellId="0" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.74609375" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3342,7 +3342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="6" t="s">
         <v>141</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="6" t="s">
         <v>141</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>160</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Pairs with given sum in DLL
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1709,21 +1709,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C159" activeCellId="0" sqref="C159"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C160" activeCellId="0" sqref="C160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75390625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3364,7 +3365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="6" t="s">
         <v>141</v>
       </c>
@@ -3375,7 +3376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="6" t="s">
         <v>141</v>
       </c>
@@ -3383,7 +3384,7 @@
         <v>162</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Triplet found in DLL
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C160" activeCellId="0" sqref="C160"/>
+      <selection pane="topLeft" activeCell="C161" activeCellId="0" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3387,7 +3387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="6" t="s">
         <v>141</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>163</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Sort k sorted DLL
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1709,22 +1709,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C161" activeCellId="0" sqref="C161"/>
+      <selection pane="topLeft" activeCell="C162" activeCellId="0" sqref="C162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7578125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="114.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3387,7 +3386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="6" t="s">
         <v>141</v>
       </c>
@@ -3398,7 +3397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="6" t="s">
         <v>141</v>
       </c>
@@ -3406,7 +3405,7 @@
         <v>164</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Rotate DLL by n nodes
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C161" activeCellId="0" sqref="C161"/>
+      <selection pane="topLeft" activeCell="C163" activeCellId="0" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3398,7 +3398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="6" t="s">
         <v>141</v>
       </c>
@@ -3406,10 +3406,10 @@
         <v>164</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="6" t="s">
         <v>141</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>165</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Rotated DLL with given size
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C163" activeCellId="0" sqref="C163"/>
+      <selection pane="topLeft" activeCell="C164" activeCellId="0" sqref="C164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3420,7 +3420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="6" t="s">
         <v>141</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>166</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Sorted LL of 0 1 2
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C167" activeCellId="0" sqref="C167"/>
+      <selection pane="topLeft" activeCell="C168" activeCellId="0" sqref="C168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3464,7 +3464,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="6" t="s">
         <v>141</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>170</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Cloned a LL with next and random pointer
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -3475,7 +3475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="6" t="s">
         <v>141</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>171</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Merged K Sorted LL
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1715,8 +1715,8 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C168" activeCellId="0" sqref="C168"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B160" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C170" activeCellId="0" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3461,7 +3461,7 @@
         <v>169</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3486,7 +3486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="6" t="s">
         <v>141</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>172</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Multiplied 2 LL as a number
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1715,7 +1715,7 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B160" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C170" activeCellId="0" sqref="C170"/>
     </sheetView>
   </sheetViews>
@@ -3497,7 +3497,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="6" t="s">
         <v>141</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>173</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Deleted nodes having greater value on right
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C170" activeCellId="0" sqref="C170"/>
+      <selection pane="topLeft" activeCell="C171" activeCellId="0" sqref="C171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3508,7 +3508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="6" t="s">
         <v>141</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>174</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Gegregated even and odd
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C171" activeCellId="0" sqref="C171"/>
+      <selection pane="topLeft" activeCell="C172" activeCellId="0" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3519,7 +3519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="6" t="s">
         <v>141</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>175</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Nth node from last
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C172" activeCellId="0" sqref="C172"/>
+      <selection pane="topLeft" activeCell="C173" activeCellId="0" sqref="C173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3530,7 +3530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="6" t="s">
         <v>141</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>176</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Level order tree traversal
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1715,7 +1715,7 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B176" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B173" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C177" activeCellId="0" sqref="C177"/>
     </sheetView>
   </sheetViews>
@@ -3564,7 +3564,7 @@
         <v>179</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Reverse order binary tree traversal
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B173" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C177" activeCellId="0" sqref="C177"/>
+      <selection pane="topLeft" activeCell="C178" activeCellId="0" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3556,7 +3556,7 @@
       <c r="B176" s="9"/>
       <c r="C176" s="5"/>
     </row>
-    <row r="177" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="6" t="s">
         <v>178</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="6" t="s">
         <v>178</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>180</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Height of Binary Tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B173" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C178" activeCellId="0" sqref="C178"/>
+      <selection pane="topLeft" activeCell="C179" activeCellId="0" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3578,7 +3578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="6" t="s">
         <v>178</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>181</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Diameter of tree found
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B173" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C179" activeCellId="0" sqref="C179"/>
+      <selection pane="topLeft" activeCell="C180" activeCellId="0" sqref="C180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3589,7 +3589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="6" t="s">
         <v>178</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>182</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Preorder, Postorder & Inorder traversal through Iteration & Recursion
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B179" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C181" activeCellId="0" sqref="C181"/>
+      <selection pane="topLeft" activeCell="C184" activeCellId="0" sqref="C184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3611,7 +3611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="6" t="s">
         <v>178</v>
       </c>
@@ -3619,10 +3619,10 @@
         <v>184</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="6" t="s">
         <v>178</v>
       </c>
@@ -3630,10 +3630,10 @@
         <v>185</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="6" t="s">
         <v>178</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>186</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Top, bottom, left & right view of tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1715,8 +1715,8 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B179" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C184" activeCellId="0" sqref="C184"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B188" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C189" activeCellId="0" sqref="C189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3644,7 +3644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="6" t="s">
         <v>178</v>
       </c>
@@ -3652,10 +3652,10 @@
         <v>187</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="6" t="s">
         <v>178</v>
       </c>
@@ -3663,10 +3663,10 @@
         <v>188</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="6" t="s">
         <v>178</v>
       </c>
@@ -3674,10 +3674,10 @@
         <v>189</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="6" t="s">
         <v>178</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>190</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
ZigZag, Diagonal & Boundary Traversal Done
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1715,8 +1715,8 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B188" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C189" activeCellId="0" sqref="C189"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C191" activeCellId="0" sqref="C191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3696,7 +3696,7 @@
         <v>191</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3710,7 +3710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="6" t="s">
         <v>178</v>
       </c>
@@ -3718,10 +3718,10 @@
         <v>193</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="6" t="s">
         <v>178</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>194</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Checked a tree is balanced or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C191" activeCellId="0" sqref="C191"/>
+      <selection pane="topLeft" activeCell="C192" activeCellId="0" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3699,7 +3699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="6" t="s">
         <v>178</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>192</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Contructed Binary Tree with String having Bracket representation
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C192" activeCellId="0" sqref="C192"/>
+      <selection pane="topLeft" activeCell="C193" activeCellId="0" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3732,7 +3732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="6" t="s">
         <v>178</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>195</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Binary Tree to Doubly Linked List
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C193" activeCellId="0" sqref="C193"/>
+      <selection pane="topLeft" activeCell="C194" activeCellId="0" sqref="C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3743,7 +3743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="6" t="s">
         <v>178</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>196</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Construct Binary Tree from Inorder and Preorder Traversal
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C195" activeCellId="0" sqref="C195"/>
+      <selection pane="topLeft" activeCell="C196" activeCellId="0" sqref="C196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3765,7 +3765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="6" t="s">
         <v>178</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>198</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Min swaps req. to conv. BT to BST
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C196" activeCellId="0" sqref="C196"/>
+      <selection pane="topLeft" activeCell="C197" activeCellId="0" sqref="C197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3776,7 +3776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="6" t="s">
         <v>178</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>199</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Check BT is Sum Tree or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C197" activeCellId="0" sqref="C197"/>
+      <selection pane="topLeft" activeCell="C198" activeCellId="0" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3787,7 +3787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="6" t="s">
         <v>178</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>200</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Level of leaf nodes
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C198" activeCellId="0" sqref="C198"/>
+      <selection pane="topLeft" activeCell="C199" activeCellId="0" sqref="C199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3798,7 +3798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="6" t="s">
         <v>178</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>201</v>
       </c>
       <c r="C199" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Checked fi there is Duplicate subtrees
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C199" activeCellId="0" sqref="C199"/>
+      <selection pane="topLeft" activeCell="C200" activeCellId="0" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3809,7 +3809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="6" t="s">
         <v>178</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>202</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Checked 2 trees are mirror or not
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C200" activeCellId="0" sqref="C200"/>
+      <selection pane="topLeft" activeCell="C201" activeCellId="0" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3820,7 +3820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="6" t="s">
         <v>178</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>203</v>
       </c>
       <c r="C201" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Sum of Longest Path from root to leaf
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1715,8 +1715,8 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B189" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C201" activeCellId="0" sqref="C201"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B192" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C202" activeCellId="0" sqref="C202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3831,7 +3831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="6" t="s">
         <v>178</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>204</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Largest SubTree Sum in a Tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1715,8 +1715,8 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B192" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C202" activeCellId="0" sqref="C202"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B190" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C204" activeCellId="0" sqref="C204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3842,15 +3842,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="6" t="s">
         <v>178</v>
       </c>
       <c r="B203" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C203" s="5" t="s">
-        <v>5</v>
+      <c r="C203" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3861,7 +3861,7 @@
         <v>206</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
FindLCA, Isomorphism, K_SumPath, MaxSumNo2AdjacentNodes
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1715,8 +1715,8 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B190" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C204" activeCellId="0" sqref="C204"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B192" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C212" activeCellId="0" sqref="C212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3853,7 +3853,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="6" t="s">
         <v>178</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="6" t="s">
         <v>178</v>
       </c>
@@ -3872,10 +3872,10 @@
         <v>207</v>
       </c>
       <c r="C205" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="206" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="6" t="s">
         <v>178</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>208</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3894,10 +3894,10 @@
         <v>209</v>
       </c>
       <c r="C207" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="6" t="s">
         <v>178</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="6" t="s">
         <v>178</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>213</v>
       </c>
       <c r="C211" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>